<commit_message>
Update call summary ETL with concurrency, retry logic, and deduplication; clean up obsolete files
Major call summary ETL enhancements: concurrent category extraction, retry with exponential
backoff, result deduplication, improved document converter with blueprint workflow, updated
prompts and category configs, and comprehensive test suite. Simplified institution_id SQL
filtering across all transcript modules. Removed obsolete IT_PACKAGE, scripts, and hotfix docs.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/src/aegis/etls/call_summary/config/categories/canadian_banks_categories.xlsx
+++ b/src/aegis/etls/call_summary/config/categories/canadian_banks_categories.xlsx
@@ -491,9 +491,6 @@
           <t>Overall financial results including revenue, net income, EPS, ROE, ROA, and key performance indicators</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -516,9 +513,6 @@
           <t>Detailed breakdown of revenue streams including net interest income, non-interest income, fee income, trading revenue, and wealth management income</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -541,9 +535,6 @@
           <t>Operating expenses, cost control initiatives, efficiency ratio, compensation costs, and technology investments</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -566,9 +557,6 @@
           <t>Loan loss provisions, net charge-offs, impaired loans, coverage ratios, and credit risk indicators specific to Canadian portfolios</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -591,9 +579,6 @@
           <t>Capital ratios (CET1, Tier 1), liquidity coverage ratio, leverage ratio, OSFI requirements, and domestic stability buffer</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -616,9 +601,6 @@
           <t>Loan growth by category, commercial loans, consumer loans, Canadian mortgage portfolio, and lending pipeline</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -641,9 +623,6 @@
           <t>Deposit growth, deposit mix, funding costs, deposit betas, and Canadian retail banking trends</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -663,12 +642,24 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Performance by division including Canadian Banking, Capital Markets, Wealth Management, Insurance, and US/International operations</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+          <t>Performance by business segment — segment names vary by bank (e.g., Global Banking &amp; Markets, Wholesale Banking, Personal &amp; Commercial). Include revenue, earnings, and growth metrics for each reported division</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>BNS: Canadian Banking, International Banking, Global Banking and Markets, Global Wealth Management</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>TD: Canadian P&amp;C, U.S. Retail, Wealth &amp; Insurance, Wholesale Banking</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>RY: Personal &amp; Commercial, Capital Markets, Wealth Management, Insurance, Investor &amp; Treasury Services</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -688,12 +679,24 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Commentary on Canadian economic environment, Bank of Canada rate outlook, housing market, and provincial economic trends</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
+          <t>Commentary on Canadian economic environment, Bank of Canada rate outlook, provincial economic trends, and banking industry outlook including competitive dynamics and sector-wide earnings expectations</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Bank of Canada rate trajectory and monetary policy impact</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>GDP growth, employment trends, consumer confidence</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Industry-wide credit trends or competitive dynamics</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -713,12 +716,24 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Management guidance for future quarters, strategic priorities, growth targets, and forward-looking statements</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+          <t>Management guidance for future quarters, earnings outlook, strategic priorities, growth targets, medium-term objectives, and forward-looking statements</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Net income growth targets or ROE guidance</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Operating leverage and efficiency ratio targets</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Medium-term strategic objectives and capital deployment plans</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -741,9 +756,6 @@
           <t>OSFI regulatory changes, B-20 guidelines, stress test results, and Canadian regulatory compliance matters</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -763,12 +775,24 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Digital transformation efforts, technology investments, AI/ML initiatives, and Canadian fintech partnerships</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
+          <t>Digital transformation efforts, technology investments, AI/ML initiatives, fintech partnerships, and technology-driven productivity and operational efficiency improvements</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Digital adoption rates and online banking migration</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Technology-driven productivity gains and process automation</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Cloud migration, cybersecurity investments, data analytics capabilities</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -791,9 +815,6 @@
           <t>Canadian housing market exposure, mortgage portfolio quality, HELOC performance, and regional real estate trends</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -816,9 +837,6 @@
           <t>Performance and strategy for US operations, international banking, and cross-border business</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -841,9 +859,6 @@
           <t>Discussion of operational risks, credit risks, market risks, regulatory risks, climate risks, and mitigation strategies</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>